<commit_message>
small changes in variable names
</commit_message>
<xml_diff>
--- a/fbref_matchdata_rawcleaning.xlsx
+++ b/fbref_matchdata_rawcleaning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb3b67440066c8ce/Jonah/Master/2_Semester/Data_Science_Project/DS-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{930E90C4-1C38-42A5-8D90-B3C577503DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{930E90C4-1C38-42A5-8D90-B3C577503DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70509204-B023-404D-91B9-53862B5F494A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{975DDA43-B140-452B-9C48-2BE8E7BE5F45}"/>
   </bookViews>
@@ -1019,30 +1019,15 @@
     <t>Squad ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Variable </t>
-  </si>
-  <si>
-    <t>Definiton/Description</t>
-  </si>
-  <si>
-    <t>Data Type</t>
-  </si>
-  <si>
     <t>Penalty Kicks Attempted against Team</t>
   </si>
   <si>
-    <t>Drop</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
     <t>False</t>
   </si>
   <si>
-    <t>Drop Justification</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -1053,6 +1038,21 @@
   </si>
   <si>
     <t>Duplicate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable </t>
+  </si>
+  <si>
+    <t>definiton_slash_description</t>
+  </si>
+  <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>drop_before_merge</t>
+  </si>
+  <si>
+    <t>drop_justification</t>
   </si>
 </sst>
 </file>
@@ -1109,11 +1109,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1130,6 +1129,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1432,33 +1435,33 @@
   <dimension ref="A1:E171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.7265625" customWidth="1"/>
+    <col min="1" max="1" width="55.6328125" customWidth="1"/>
     <col min="2" max="2" width="86.1796875" customWidth="1"/>
     <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="5" max="5" width="19.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>334</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1469,10 +1472,10 @@
         <v>319</v>
       </c>
       <c r="D2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1483,10 +1486,10 @@
         <v>320</v>
       </c>
       <c r="D3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E3" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1497,10 +1500,10 @@
         <v>170</v>
       </c>
       <c r="D4" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E4" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1511,10 +1514,10 @@
         <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E5" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1525,10 +1528,10 @@
         <v>321</v>
       </c>
       <c r="D6" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E6" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1539,10 +1542,10 @@
         <v>322</v>
       </c>
       <c r="D7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E7" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1553,24 +1556,24 @@
         <v>172</v>
       </c>
       <c r="D8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>173</v>
       </c>
       <c r="D9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E9" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1581,52 +1584,52 @@
         <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E10" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E11" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>176</v>
       </c>
       <c r="D12" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E12" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>177</v>
       </c>
       <c r="D13" t="s">
+        <v>328</v>
+      </c>
+      <c r="E13" t="s">
         <v>333</v>
-      </c>
-      <c r="E13" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1637,10 +1640,10 @@
         <v>178</v>
       </c>
       <c r="D14" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E14" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1651,10 +1654,10 @@
         <v>179</v>
       </c>
       <c r="D15" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E15" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1665,10 +1668,10 @@
         <v>180</v>
       </c>
       <c r="D16" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E16" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1679,38 +1682,38 @@
         <v>181</v>
       </c>
       <c r="D17" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E17" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>335</v>
+      <c r="B18" t="s">
+        <v>330</v>
       </c>
       <c r="D18" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E18" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>335</v>
+      <c r="B19" t="s">
+        <v>330</v>
       </c>
       <c r="D19" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E19" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1721,10 +1724,10 @@
         <v>323</v>
       </c>
       <c r="D20" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E20" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1735,10 +1738,10 @@
         <v>324</v>
       </c>
       <c r="D21" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E21" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1749,10 +1752,10 @@
         <v>326</v>
       </c>
       <c r="D22" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E22" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1763,10 +1766,10 @@
         <v>325</v>
       </c>
       <c r="D23" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E23" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1774,13 +1777,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D24" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E24" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1791,10 +1794,10 @@
         <v>182</v>
       </c>
       <c r="D25" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E25" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1805,10 +1808,10 @@
         <v>183</v>
       </c>
       <c r="D26" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E26" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1819,10 +1822,10 @@
         <v>184</v>
       </c>
       <c r="D27" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E27" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1833,10 +1836,10 @@
         <v>185</v>
       </c>
       <c r="D28" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E28" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1847,10 +1850,10 @@
         <v>186</v>
       </c>
       <c r="D29" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E29" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1861,10 +1864,10 @@
         <v>187</v>
       </c>
       <c r="D30" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E30" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1875,10 +1878,10 @@
         <v>188</v>
       </c>
       <c r="D31" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E31" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1889,52 +1892,52 @@
         <v>189</v>
       </c>
       <c r="D32" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E32" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" t="s">
         <v>190</v>
       </c>
       <c r="D33" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E33" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" t="s">
         <v>191</v>
       </c>
       <c r="D34" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E34" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" t="s">
         <v>175</v>
       </c>
       <c r="D35" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E35" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1945,10 +1948,10 @@
         <v>192</v>
       </c>
       <c r="D36" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E36" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1959,10 +1962,10 @@
         <v>193</v>
       </c>
       <c r="D37" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E37" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1973,10 +1976,10 @@
         <v>194</v>
       </c>
       <c r="D38" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E38" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1987,10 +1990,10 @@
         <v>195</v>
       </c>
       <c r="D39" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E39" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -2001,24 +2004,24 @@
         <v>196</v>
       </c>
       <c r="D40" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E40" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" t="s">
         <v>173</v>
       </c>
       <c r="D41" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E41" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -2029,10 +2032,10 @@
         <v>197</v>
       </c>
       <c r="D42" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E42" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -2043,10 +2046,10 @@
         <v>198</v>
       </c>
       <c r="D43" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E43" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -2057,10 +2060,10 @@
         <v>199</v>
       </c>
       <c r="D44" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E44" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -2071,10 +2074,10 @@
         <v>201</v>
       </c>
       <c r="D45" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E45" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -2085,24 +2088,24 @@
         <v>200</v>
       </c>
       <c r="D46" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E46" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>330</v>
+      <c r="B47" t="s">
+        <v>327</v>
       </c>
       <c r="D47" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E47" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -2113,10 +2116,10 @@
         <v>202</v>
       </c>
       <c r="D48" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E48" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -2127,10 +2130,10 @@
         <v>203</v>
       </c>
       <c r="D49" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E49" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -2141,10 +2144,10 @@
         <v>204</v>
       </c>
       <c r="D50" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E50" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -2155,10 +2158,10 @@
         <v>205</v>
       </c>
       <c r="D51" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E51" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -2169,10 +2172,10 @@
         <v>206</v>
       </c>
       <c r="D52" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E52" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
@@ -2183,10 +2186,10 @@
         <v>207</v>
       </c>
       <c r="D53" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E53" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -2197,10 +2200,10 @@
         <v>208</v>
       </c>
       <c r="D54" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E54" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -2211,10 +2214,10 @@
         <v>209</v>
       </c>
       <c r="D55" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E55" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -2225,10 +2228,10 @@
         <v>212</v>
       </c>
       <c r="D56" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E56" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
@@ -2239,10 +2242,10 @@
         <v>210</v>
       </c>
       <c r="D57" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E57" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
@@ -2253,10 +2256,10 @@
         <v>211</v>
       </c>
       <c r="D58" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E58" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
@@ -2267,10 +2270,10 @@
         <v>213</v>
       </c>
       <c r="D59" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E59" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
@@ -2281,10 +2284,10 @@
         <v>217</v>
       </c>
       <c r="D60" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E60" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
@@ -2295,10 +2298,10 @@
         <v>214</v>
       </c>
       <c r="D61" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E61" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -2309,10 +2312,10 @@
         <v>215</v>
       </c>
       <c r="D62" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E62" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
@@ -2323,10 +2326,10 @@
         <v>216</v>
       </c>
       <c r="D63" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E63" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -2337,10 +2340,10 @@
         <v>218</v>
       </c>
       <c r="D64" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E64" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -2351,38 +2354,38 @@
         <v>219</v>
       </c>
       <c r="D65" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E65" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" t="s">
         <v>220</v>
       </c>
       <c r="D66" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E66" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>65</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" t="s">
         <v>221</v>
       </c>
       <c r="D67" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E67" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -2393,10 +2396,10 @@
         <v>222</v>
       </c>
       <c r="D68" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E68" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -2407,10 +2410,10 @@
         <v>224</v>
       </c>
       <c r="D69" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E69" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
@@ -2421,10 +2424,10 @@
         <v>223</v>
       </c>
       <c r="D70" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E70" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
@@ -2435,10 +2438,10 @@
         <v>225</v>
       </c>
       <c r="D71" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E71" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
@@ -2449,10 +2452,10 @@
         <v>226</v>
       </c>
       <c r="D72" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E72" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -2463,10 +2466,10 @@
         <v>227</v>
       </c>
       <c r="D73" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E73" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
@@ -2477,10 +2480,10 @@
         <v>228</v>
       </c>
       <c r="D74" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E74" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -2491,10 +2494,10 @@
         <v>229</v>
       </c>
       <c r="D75" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E75" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
@@ -2505,10 +2508,10 @@
         <v>230</v>
       </c>
       <c r="D76" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E76" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
@@ -2519,10 +2522,10 @@
         <v>232</v>
       </c>
       <c r="D77" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E77" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
@@ -2533,10 +2536,10 @@
         <v>231</v>
       </c>
       <c r="D78" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E78" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
@@ -2547,10 +2550,10 @@
         <v>233</v>
       </c>
       <c r="D79" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E79" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -2561,10 +2564,10 @@
         <v>234</v>
       </c>
       <c r="D80" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E80" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
@@ -2575,10 +2578,10 @@
         <v>235</v>
       </c>
       <c r="D81" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E81" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
@@ -2589,10 +2592,10 @@
         <v>236</v>
       </c>
       <c r="D82" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E82" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
@@ -2603,10 +2606,10 @@
         <v>237</v>
       </c>
       <c r="D83" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E83" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
@@ -2617,10 +2620,10 @@
         <v>238</v>
       </c>
       <c r="D84" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E84" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
@@ -2631,10 +2634,10 @@
         <v>239</v>
       </c>
       <c r="D85" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E85" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
@@ -2645,38 +2648,38 @@
         <v>240</v>
       </c>
       <c r="D86" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E86" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" t="s">
         <v>299</v>
       </c>
       <c r="D87" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E87" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" t="s">
         <v>221</v>
       </c>
       <c r="D88" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E88" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
@@ -2687,10 +2690,10 @@
         <v>241</v>
       </c>
       <c r="D89" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E89" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
@@ -2701,10 +2704,10 @@
         <v>242</v>
       </c>
       <c r="D90" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E90" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
@@ -2715,10 +2718,10 @@
         <v>243</v>
       </c>
       <c r="D91" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E91" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
@@ -2729,10 +2732,10 @@
         <v>244</v>
       </c>
       <c r="D92" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E92" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
@@ -2743,24 +2746,24 @@
         <v>245</v>
       </c>
       <c r="D93" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E93" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" t="s">
         <v>246</v>
       </c>
       <c r="D94" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E94" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
@@ -2771,10 +2774,10 @@
         <v>247</v>
       </c>
       <c r="D95" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E95" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
@@ -2785,10 +2788,10 @@
         <v>248</v>
       </c>
       <c r="D96" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E96" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
@@ -2799,10 +2802,10 @@
         <v>249</v>
       </c>
       <c r="D97" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E97" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
@@ -2813,10 +2816,10 @@
         <v>250</v>
       </c>
       <c r="D98" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E98" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
@@ -2827,24 +2830,24 @@
         <v>251</v>
       </c>
       <c r="D99" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E99" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" t="s">
         <v>220</v>
       </c>
       <c r="D100" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E100" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
@@ -2855,10 +2858,10 @@
         <v>252</v>
       </c>
       <c r="D101" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E101" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
@@ -2869,10 +2872,10 @@
         <v>253</v>
       </c>
       <c r="D102" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E102" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
@@ -2883,10 +2886,10 @@
         <v>254</v>
       </c>
       <c r="D103" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E103" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
@@ -2897,10 +2900,10 @@
         <v>255</v>
       </c>
       <c r="D104" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E104" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
@@ -2911,10 +2914,10 @@
         <v>256</v>
       </c>
       <c r="D105" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E105" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
@@ -2925,10 +2928,10 @@
         <v>257</v>
       </c>
       <c r="D106" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E106" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
@@ -2939,10 +2942,10 @@
         <v>258</v>
       </c>
       <c r="D107" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E107" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
@@ -2953,10 +2956,10 @@
         <v>259</v>
       </c>
       <c r="D108" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E108" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
@@ -2967,10 +2970,10 @@
         <v>260</v>
       </c>
       <c r="D109" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E109" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
@@ -2981,10 +2984,10 @@
         <v>261</v>
       </c>
       <c r="D110" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E110" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
@@ -2995,10 +2998,10 @@
         <v>262</v>
       </c>
       <c r="D111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E111" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
@@ -3009,10 +3012,10 @@
         <v>263</v>
       </c>
       <c r="D112" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E112" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
@@ -3023,10 +3026,10 @@
         <v>264</v>
       </c>
       <c r="D113" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E113" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
@@ -3037,10 +3040,10 @@
         <v>265</v>
       </c>
       <c r="D114" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E114" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
@@ -3051,10 +3054,10 @@
         <v>266</v>
       </c>
       <c r="D115" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E115" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
@@ -3065,10 +3068,10 @@
         <v>267</v>
       </c>
       <c r="D116" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E116" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
@@ -3079,24 +3082,24 @@
         <v>268</v>
       </c>
       <c r="D117" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E117" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" t="s">
         <v>269</v>
       </c>
       <c r="D118" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E118" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
@@ -3107,10 +3110,10 @@
         <v>270</v>
       </c>
       <c r="D119" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E119" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
@@ -3121,10 +3124,10 @@
         <v>271</v>
       </c>
       <c r="D120" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E120" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
@@ -3135,10 +3138,10 @@
         <v>272</v>
       </c>
       <c r="D121" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E121" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
@@ -3149,10 +3152,10 @@
         <v>273</v>
       </c>
       <c r="D122" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E122" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
@@ -3163,10 +3166,10 @@
         <v>274</v>
       </c>
       <c r="D123" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E123" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
@@ -3177,10 +3180,10 @@
         <v>275</v>
       </c>
       <c r="D124" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E124" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
@@ -3191,10 +3194,10 @@
         <v>276</v>
       </c>
       <c r="D125" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E125" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
@@ -3205,10 +3208,10 @@
         <v>277</v>
       </c>
       <c r="D126" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E126" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
@@ -3219,10 +3222,10 @@
         <v>278</v>
       </c>
       <c r="D127" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E127" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
@@ -3233,24 +3236,24 @@
         <v>279</v>
       </c>
       <c r="D128" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E128" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>127</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B129" t="s">
         <v>280</v>
       </c>
       <c r="D129" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E129" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
@@ -3261,10 +3264,10 @@
         <v>281</v>
       </c>
       <c r="D130" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E130" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
@@ -3275,10 +3278,10 @@
         <v>282</v>
       </c>
       <c r="D131" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E131" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
@@ -3289,24 +3292,24 @@
         <v>283</v>
       </c>
       <c r="D132" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E132" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>131</v>
       </c>
-      <c r="B133" s="3" t="s">
+      <c r="B133" t="s">
         <v>177</v>
       </c>
       <c r="D133" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E133" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
@@ -3317,10 +3320,10 @@
         <v>284</v>
       </c>
       <c r="D134" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E134" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
@@ -3331,10 +3334,10 @@
         <v>285</v>
       </c>
       <c r="D135" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E135" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
@@ -3345,10 +3348,10 @@
         <v>286</v>
       </c>
       <c r="D136" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E136" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
@@ -3359,10 +3362,10 @@
         <v>287</v>
       </c>
       <c r="D137" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E137" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
@@ -3373,10 +3376,10 @@
         <v>289</v>
       </c>
       <c r="D138" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E138" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
@@ -3387,10 +3390,10 @@
         <v>288</v>
       </c>
       <c r="D139" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E139" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
@@ -3401,10 +3404,10 @@
         <v>290</v>
       </c>
       <c r="D140" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E140" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
@@ -3415,10 +3418,10 @@
         <v>291</v>
       </c>
       <c r="D141" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E141" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
@@ -3429,10 +3432,10 @@
         <v>292</v>
       </c>
       <c r="D142" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E142" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
@@ -3443,10 +3446,10 @@
         <v>293</v>
       </c>
       <c r="D143" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E143" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
@@ -3457,10 +3460,10 @@
         <v>294</v>
       </c>
       <c r="D144" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E144" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
@@ -3471,10 +3474,10 @@
         <v>295</v>
       </c>
       <c r="D145" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E145" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
@@ -3485,10 +3488,10 @@
         <v>296</v>
       </c>
       <c r="D146" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E146" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
@@ -3499,10 +3502,10 @@
         <v>297</v>
       </c>
       <c r="D147" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E147" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
@@ -3513,10 +3516,10 @@
         <v>298</v>
       </c>
       <c r="D148" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E148" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
@@ -3527,10 +3530,10 @@
         <v>300</v>
       </c>
       <c r="D149" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E149" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
@@ -3541,10 +3544,10 @@
         <v>301</v>
       </c>
       <c r="D150" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E150" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
@@ -3555,10 +3558,10 @@
         <v>302</v>
       </c>
       <c r="D151" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E151" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
@@ -3569,10 +3572,10 @@
         <v>303</v>
       </c>
       <c r="D152" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E152" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
@@ -3583,10 +3586,10 @@
         <v>304</v>
       </c>
       <c r="D153" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E153" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
@@ -3597,24 +3600,24 @@
         <v>305</v>
       </c>
       <c r="D154" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E154" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>153</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B155" t="s">
         <v>299</v>
       </c>
       <c r="D155" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E155" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
@@ -3625,10 +3628,10 @@
         <v>306</v>
       </c>
       <c r="D156" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E156" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
@@ -3639,10 +3642,10 @@
         <v>307</v>
       </c>
       <c r="D157" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E157" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
@@ -3653,10 +3656,10 @@
         <v>308</v>
       </c>
       <c r="D158" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E158" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
@@ -3667,10 +3670,10 @@
         <v>309</v>
       </c>
       <c r="D159" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E159" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
@@ -3681,164 +3684,164 @@
         <v>311</v>
       </c>
       <c r="D160" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E160" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>159</v>
       </c>
-      <c r="B161" s="3" t="s">
+      <c r="B161" t="s">
         <v>310</v>
       </c>
       <c r="D161" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E161" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>160</v>
       </c>
-      <c r="B162" s="3" t="s">
+      <c r="B162" t="s">
         <v>246</v>
       </c>
       <c r="D162" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E162" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>161</v>
       </c>
-      <c r="B163" s="3" t="s">
+      <c r="B163" t="s">
         <v>280</v>
       </c>
       <c r="D163" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E163" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>162</v>
       </c>
-      <c r="B164" s="3" t="s">
+      <c r="B164" t="s">
         <v>269</v>
       </c>
       <c r="D164" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E164" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>163</v>
       </c>
-      <c r="B165" s="3" t="s">
+      <c r="B165" t="s">
         <v>312</v>
       </c>
       <c r="D165" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E165" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>164</v>
       </c>
-      <c r="B166" s="3" t="s">
+      <c r="B166" t="s">
         <v>313</v>
       </c>
       <c r="D166" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E166" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>165</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="B167" t="s">
         <v>314</v>
       </c>
       <c r="D167" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E167" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>166</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B168" t="s">
         <v>315</v>
       </c>
       <c r="D168" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E168" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>167</v>
       </c>
-      <c r="B169" s="3" t="s">
+      <c r="B169" t="s">
         <v>317</v>
       </c>
       <c r="D169" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E169" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>168</v>
       </c>
-      <c r="B170" s="3" t="s">
+      <c r="B170" t="s">
         <v>316</v>
       </c>
       <c r="D170" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E170" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>169</v>
       </c>
-      <c r="B171" s="3" t="s">
+      <c r="B171" t="s">
         <v>318</v>
       </c>
       <c r="D171" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E171" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>